<commit_message>
COD02 Complete export save as
</commit_message>
<xml_diff>
--- a/47全國技能_北區/02 SoftwareDesign/Data/CO02/data.xlsx
+++ b/47全國技能_北區/02 SoftwareDesign/Data/CO02/data.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="1545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="1545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="台北市自行車旅遊景點" sheetId="6" r:id="rId1"/>
-    <sheet name="新北市自行車旅遊景點" sheetId="4" r:id="rId2"/>
-    <sheet name="高雄市自行車旅遊景點" sheetId="1" r:id="rId3"/>
+    <sheet name="Test" sheetId="7" r:id="rId2"/>
+    <sheet name="新北市自行車旅遊景點" sheetId="4" r:id="rId3"/>
+    <sheet name="高雄市自行車旅遊景點" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="1946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="1946">
   <si>
     <t>代碼</t>
   </si>
@@ -6278,8 +6279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -10240,6 +10241,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D2" s="2">
+        <v>25.0408578889</v>
+      </c>
+      <c r="E2" s="2">
+        <v>121.56790444400001</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F367"/>
   <sheetViews>
@@ -17604,7 +17662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>